<commit_message>
Add some keyword methods
</commit_message>
<xml_diff>
--- a/src/test/java/com/bat/xlsx/suitea.xlsx
+++ b/src/test/java/com/bat/xlsx/suitea.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Keywords" sheetId="2" r:id="rId1"/>
-    <sheet name="TestA" sheetId="1" r:id="rId2"/>
+    <sheet name="Test Cases" sheetId="3" r:id="rId1"/>
+    <sheet name="Keywords" sheetId="2" r:id="rId2"/>
+    <sheet name="TestA" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="35">
   <si>
     <t>Runmode</t>
   </si>
@@ -127,6 +128,12 @@
   </si>
   <si>
     <t>Data_key</t>
+  </si>
+  <si>
+    <t>TestB</t>
+  </si>
+  <si>
+    <t>TestC</t>
   </si>
 </sst>
 </file>
@@ -483,6 +490,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -655,11 +712,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add screen shots and proceed on failure checking
</commit_message>
<xml_diff>
--- a/src/test/java/com/bat/xlsx/suitea.xlsx
+++ b/src/test/java/com/bat/xlsx/suitea.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="3" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="36">
   <si>
     <t>Runmode</t>
   </si>
@@ -134,6 +134,9 @@
   </si>
   <si>
     <t>TestC</t>
+  </si>
+  <si>
+    <t>Proceed_on_fail</t>
   </si>
 </sst>
 </file>
@@ -492,7 +495,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -540,10 +543,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,7 +559,7 @@
     <col min="6" max="8" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -572,8 +575,11 @@
       <c r="E1" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -584,7 +590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -594,8 +600,11 @@
       <c r="D3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -608,8 +617,11 @@
       <c r="E4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -619,8 +631,11 @@
       <c r="D5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -630,8 +645,11 @@
       <c r="D6" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -641,8 +659,11 @@
       <c r="D7" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -652,8 +673,11 @@
       <c r="D8" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -664,7 +688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -678,7 +702,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -692,7 +716,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>

</xml_diff>